<commit_message>
adding cleaned mastercard data
</commit_message>
<xml_diff>
--- a/Mastercard/Data/mastercard_data.xlsx
+++ b/Mastercard/Data/mastercard_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marijkevandergeer/Desktop/Biokind/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marijkevandergeer/Documents/GitHub/biokind_dspg23/Mastercard/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67307946-9F35-E24D-B248-B19D3407965E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D7E52C-4896-A44E-BF04-25BAB2648A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{9A0062DC-6EBF-D044-82DD-2D301B744A46}"/>
   </bookViews>
@@ -41,19 +41,19 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Donation-Index-Amount-Y/Y-Growth</t>
+    <t>Donation</t>
   </si>
   <si>
-    <t>Donation-Index-Amount-3-Month-Moving-Avg</t>
+    <t>Number_Donations_Growth</t>
   </si>
   <si>
-    <t>Number-of-Donations-Y/Y-Growth</t>
+    <t>Donation_Index_Growth</t>
   </si>
   <si>
-    <t>Average-Donation-Size-Y/Y-Growth</t>
+    <t>Donation_Index_3_Month_Avg</t>
   </si>
   <si>
-    <t>Donation</t>
+    <t>Avg_Donation_Size_Growth</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,24 +485,24 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">

</xml_diff>